<commit_message>
beh-maker 추가 / password 설정 추가
</commit_message>
<xml_diff>
--- a/data/output/client_15/conversation_client_15.xlsx
+++ b/data/output/client_15/conversation_client_15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>human</t>
   </si>
@@ -22,22 +22,28 @@
     <t>simulated client</t>
   </si>
   <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>I'm Dr.Lee</t>
-  </si>
-  <si>
-    <t>What brings you here?</t>
-  </si>
-  <si>
-    <t>Hello. How are you feeling today?</t>
-  </si>
-  <si>
-    <t>Oh, hi Dr. Lee. Um, I'm Jin-ah. I guess I'm... okay? I'm not really sure.</t>
-  </si>
-  <si>
-    <t>I've been feeling really down for quite a while now. It started back in early 2021, and it just hasn't gotten better. Lately, it's been worse, and I can't seem to shake this sense of hopelessness. Also, I can't sleep well at all. It's like my mind won't let me rest.</t>
+    <t>Hello, I'm Dr.Lee</t>
+  </si>
+  <si>
+    <t>What's your name?</t>
+  </si>
+  <si>
+    <t>Okay, Jin-ah. What brings you here?</t>
+  </si>
+  <si>
+    <t>Tell me about you more</t>
+  </si>
+  <si>
+    <t>Hi, Dr. Lee.</t>
+  </si>
+  <si>
+    <t>I'm Jin-ah.</t>
+  </si>
+  <si>
+    <t>I've been feeling really down for a long time. It's not getting any better, and lately, I can't seem to sleep either. I just... I don't know what to do anymore.</t>
+  </si>
+  <si>
+    <t>Well, I'm 24 years old, and I'm a graduate student. I live in Seoul with my family. I have a younger brother. My mom has had her own struggles with depression, and my dad has hypertension. I've been dealing with these feelings of sadness since early 2021, and it's just been getting worse. I started having trouble sleeping around mid-2022, and now it's almost impossible to get a good night's rest. I'm on antidepressants, but they don't seem to be helping much.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -422,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -430,7 +436,15 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>